<commit_message>
Fix bug in dict.xlsx and make_tidy.py that caused validation sequences to all use contiguous codes. Do validation with second-generation sequences.
</commit_message>
<xml_diff>
--- a/dict.xlsx
+++ b/dict.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="2560" windowWidth="21600" windowHeight="14660" tabRatio="500"/>
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t>N1</t>
   </si>
@@ -657,20 +657,49 @@
   <si>
     <t>C1C2</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n2_2</t>
+  </si>
+  <si>
+    <t>n1_2</t>
+  </si>
+  <si>
+    <t>n3_2</t>
+  </si>
+  <si>
+    <t>c1_2</t>
+  </si>
+  <si>
+    <t>n4_2</t>
+  </si>
+  <si>
+    <t>n5_2</t>
+  </si>
+  <si>
+    <t>n6_2</t>
+  </si>
+  <si>
+    <t>c2_2</t>
+  </si>
+  <si>
+    <t>n7_2</t>
+  </si>
+  <si>
+    <t>c3_2</t>
+  </si>
+  <si>
+    <t>n8_2</t>
+  </si>
+  <si>
+    <t>c4_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -684,31 +713,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -720,20 +743,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1056,15 +1091,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:B210"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B222"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
@@ -2749,12 +2783,108 @@
         <v>1112333322</v>
       </c>
     </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B211" s="1">
+        <v>2233331232</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B212" s="1">
+        <v>2233333232</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B213" s="1">
+        <v>3233331232</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B214" s="1">
+        <v>3333332331</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B215" s="1">
+        <v>1322222323</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B216" s="1">
+        <v>3322223323</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B217" s="1">
+        <v>3231333231</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B218" s="1">
+        <v>2213323323</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B219" s="1">
+        <v>1231331111</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" s="1">
+        <v>3333332331</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B221" s="1">
+        <v>2333233333</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B222" s="1">
+        <v>3333332332</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Fix codes for c1c2 and cschrimson in dict.xlsx. Update some models and dfs accordingly.
</commit_message>
<xml_diff>
--- a/dict.xlsx
+++ b/dict.xlsx
@@ -743,8 +743,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -758,13 +764,19 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1094,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B222"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1123,16 +1135,16 @@
       <c r="A3" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="3">
-        <v>3333333333</v>
+      <c r="B3" s="1">
+        <v>2222222222</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="1">
-        <v>2222222222</v>
+      <c r="B4" s="3">
+        <v>3333333333</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
Expand sample space and contacts so dict so that sequences can be generated for chimeras with CbChR1 or CsCbChR1 as parents.
</commit_message>
<xml_diff>
--- a/dict.xlsx
+++ b/dict.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
   <si>
     <t>N1</t>
   </si>
@@ -693,6 +693,12 @@
   </si>
   <si>
     <t>c4_2</t>
+  </si>
+  <si>
+    <t>cbchr1</t>
+  </si>
+  <si>
+    <t>cscbchr1</t>
   </si>
 </sst>
 </file>
@@ -1104,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B222"/>
+  <dimension ref="A1:B224"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2889,6 +2895,22 @@
       </c>
       <c r="B222" s="1">
         <v>3333332332</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B223" s="1">
+        <v>4444444444</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B224" s="1">
+        <v>5555555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>